<commit_message>
Updates to excel to open on another pc
</commit_message>
<xml_diff>
--- a/data/vulnerabilities.xlsx
+++ b/data/vulnerabilities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\Uni\Talentos\LLM-and-ODC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A062C7-7C83-42B6-A823-E630960EFC66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B025C1D-037D-420C-A0CE-5021976A79D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A00165BD-DFB3-BD4B-9391-7BF7A583E416}"/>
   </bookViews>
@@ -22,10 +22,10 @@
     <sheet name="cve_title" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Vulnerabilities!$A$2:$H$269</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Vulnerabilities!$A$2:$H$268</definedName>
     <definedName name="cve_title_1" localSheetId="6">cve_title!$A$1:$B$164</definedName>
     <definedName name="patch_files_info" localSheetId="3">patch_files_info!$A$1:$G$706</definedName>
-    <definedName name="relevant_vuln" localSheetId="0">Vulnerabilities!$A$3:$E$269</definedName>
+    <definedName name="relevant_vuln" localSheetId="0">Vulnerabilities!$A$3:$E$268</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5606" uniqueCount="1521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5597" uniqueCount="1521">
   <si>
     <t>V_ID</t>
   </si>
@@ -4657,7 +4657,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4718,6 +4718,21 @@
       <u/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4933,7 +4948,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5011,16 +5026,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -5846,7 +5862,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="José Alexandre D'Abruzzo Pereira" refreshedDate="44314.783292361113" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="238" xr:uid="{7517D783-7974-CB4C-8E79-0ECB0454C552}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A2:H269" sheet="Vulnerabilities"/>
+    <worksheetSource ref="A2:H268" sheet="Vulnerabilities"/>
   </cacheSource>
   <cacheFields count="11">
     <cacheField name="V_ID" numFmtId="0">
@@ -5906,7 +5922,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="José Alexandre D'Abruzzo Pereira" refreshedDate="44314.89997766204" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="238" xr:uid="{681B9B8C-63E4-AE4F-90B3-41EA5175267F}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A2:G269" sheet="Vulnerabilities"/>
+    <worksheetSource ref="A2:G268" sheet="Vulnerabilities"/>
   </cacheSource>
   <cacheFields count="11">
     <cacheField name="V_ID" numFmtId="0">
@@ -18517,93 +18533,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FA04E8B4-5D2A-6547-9536-E6B83133873B}" name="Tabela Dinâmica4" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A34:F40" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="11">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="10"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Contagem de Defect Qualifier" fld="10" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{816AEB3D-4CC5-3D43-8CBF-7375092873C9}" name="Tabela Dinâmica3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A21:F29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="11">
@@ -18698,7 +18627,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{876C571E-2282-4D43-8D98-53DB7CC78851}" name="Tabela Dinâmica2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="11">
@@ -18780,6 +18709,93 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Contagem de Defect Type" fld="8" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FA04E8B4-5D2A-6547-9536-E6B83133873B}" name="Tabela Dinâmica4" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A34:F40" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="11">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="10"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Contagem de Defect Qualifier" fld="10" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -20446,11 +20462,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ED6079-E8B5-6640-BD42-6CBFE9D43206}">
-  <dimension ref="A1:N269"/>
+  <dimension ref="A1:N268"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="79" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A256" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K268" sqref="K268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -20470,10 +20486,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="F1" s="75" t="s">
+      <c r="F1" s="77" t="s">
         <v>1505</v>
       </c>
-      <c r="G1" s="76"/>
+      <c r="G1" s="78"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -21432,17 +21448,17 @@
         <v>538</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="77" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="77" t="s">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="77" t="s">
+      <c r="B26" t="s">
         <v>1509</v>
       </c>
-      <c r="C26" s="77" t="s">
+      <c r="C26" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="77" t="s">
+      <c r="D26" t="s">
         <v>480</v>
       </c>
       <c r="E26" s="4" t="s">
@@ -21454,35 +21470,35 @@
       <c r="G26" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="H26" s="77">
+      <c r="H26">
         <f>_xlfn.XLOOKUP(E26,commit_num_files!A$2:A$319,commit_num_files!B$2:B$319)</f>
         <v>7</v>
       </c>
-      <c r="I26" s="77" t="str">
+      <c r="I26" t="str">
         <f>_xlfn.XLOOKUP(C26,cve_title!A$2:A$164,cve_title!B$2:B$164)</f>
         <v>Mozilla Firefox before 3.6.18 and 4.x through 4.0.1, Thunderbird before 3.1.11, and SeaMonkey through 2.0.14 allow remote attackers to cause a denial of service (memory corruption and application crash) or possibly execute arbitrary code via a multipart/x-mixed-replace image.</v>
       </c>
       <c r="K26" s="36" t="s">
         <v>1349</v>
       </c>
-      <c r="L26" s="77" t="s">
+      <c r="L26" t="s">
         <v>1460</v>
       </c>
-      <c r="N26" s="77" t="s">
+      <c r="N26" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A27" s="77" t="s">
+      <c r="A27" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="77" t="s">
+      <c r="B27" t="s">
         <v>1509</v>
       </c>
-      <c r="C27" s="77" t="s">
+      <c r="C27" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="77" t="s">
+      <c r="D27" t="s">
         <v>480</v>
       </c>
       <c r="E27" s="4" t="s">
@@ -21494,23 +21510,21 @@
       <c r="G27" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="H27" s="77">
+      <c r="H27">
         <f>_xlfn.XLOOKUP(E27,commit_num_files!A$2:A$319,commit_num_files!B$2:B$319)</f>
         <v>7</v>
       </c>
-      <c r="I27" s="77" t="str">
+      <c r="I27" t="str">
         <f>_xlfn.XLOOKUP(C27,cve_title!A$2:A$164,cve_title!B$2:B$164)</f>
         <v>Mozilla Firefox before 3.6.18 and 4.x through 4.0.1, Thunderbird before 3.1.11, and SeaMonkey through 2.0.14 allow remote attackers to cause a denial of service (memory corruption and application crash) or possibly execute arbitrary code via a multipart/x-mixed-replace image.</v>
       </c>
-      <c r="J27" s="77"/>
       <c r="K27" s="36" t="s">
         <v>1349</v>
       </c>
-      <c r="L27" s="77" t="s">
+      <c r="L27" t="s">
         <v>1460</v>
       </c>
-      <c r="M27" s="77"/>
-      <c r="N27" s="77" t="s">
+      <c r="N27" t="s">
         <v>540</v>
       </c>
     </row>
@@ -30837,7 +30851,7 @@
         <f>_xlfn.XLOOKUP(E261,commit_num_files!A$2:A$319,commit_num_files!B$2:B$319)</f>
         <v>1</v>
       </c>
-      <c r="I261" t="str">
+      <c r="I261" s="59" t="str">
         <f>_xlfn.XLOOKUP(C261,cve_title!A$2:A$164,cve_title!B$2:B$164)</f>
         <v>Array index error in the tcm_vhost_make_tpg function in drivers/vhost/scsi.c in the Linux kernel before 4.0 might allow guest OS users to cause a denial of service (memory corruption) or possibly have unspecified other impact via a crafted VHOST_SCSI_SET_ENDPOINT ioctl call.  NOTE: the affected function was renamed to vhost_scsi_make_tpg before the vulnerability was announced.</v>
       </c>
@@ -30851,184 +30865,185 @@
       <c r="M261" s="59"/>
       <c r="N261" s="59"/>
     </row>
-    <row r="262" spans="1:14" s="8" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A262" s="78" t="s">
+    <row r="262" spans="1:14" s="79" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A262" s="79" t="s">
         <v>465</v>
       </c>
-      <c r="B262" s="78" t="s">
+      <c r="B262" s="79" t="s">
         <v>1511</v>
       </c>
-      <c r="C262" s="78" t="s">
+      <c r="C262" s="79" t="s">
         <v>466</v>
       </c>
-      <c r="D262" s="78" t="s">
+      <c r="D262" s="79" t="s">
         <v>487</v>
       </c>
-      <c r="E262" s="79" t="s">
+      <c r="E262" s="80" t="s">
         <v>467</v>
       </c>
-      <c r="F262" s="78" t="s">
-        <v>498</v>
-      </c>
-      <c r="G262" s="79" t="s">
-        <v>502</v>
-      </c>
-      <c r="H262" s="78">
-        <v>1</v>
-      </c>
-      <c r="I262" s="8" t="str">
+      <c r="F262" s="79" t="s">
+        <v>506</v>
+      </c>
+      <c r="G262" s="80" t="s">
+        <v>503</v>
+      </c>
+      <c r="H262" s="79">
+        <f>_xlfn.XLOOKUP(E262,commit_num_files!A$2:A$319,commit_num_files!B$2:B$319)</f>
+        <v>1</v>
+      </c>
+      <c r="I262" s="79" t="str">
         <f>_xlfn.XLOOKUP(C262,cve_title!A$2:A$164,cve_title!B$2:B$164)</f>
         <v>Stack-based buffer overflow in the dirty video RAM tracking functionality in Xen 3.4 through 4.1 allows local HVM guest OS administrators to cause a denial of service (crash) via a large bitmap image.</v>
       </c>
-      <c r="J262" s="78"/>
-      <c r="K262" s="78" t="s">
+      <c r="K262" s="81" t="s">
         <v>1325</v>
       </c>
-      <c r="L262" s="78" t="s">
+      <c r="L262" s="79" t="s">
         <v>1460</v>
       </c>
-      <c r="M262" s="78"/>
-      <c r="N262" s="78"/>
-    </row>
-    <row r="263" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A263" s="22" t="s">
-        <v>465</v>
-      </c>
-      <c r="B263" s="22" t="s">
+    </row>
+    <row r="263" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A263" t="s">
+        <v>468</v>
+      </c>
+      <c r="B263" t="s">
         <v>1511</v>
       </c>
-      <c r="C263" s="22" t="s">
-        <v>466</v>
-      </c>
-      <c r="D263" s="22" t="s">
+      <c r="C263" t="s">
+        <v>469</v>
+      </c>
+      <c r="D263" t="s">
+        <v>491</v>
+      </c>
+      <c r="E263" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="F263" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="G263" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="H263">
+        <f>_xlfn.XLOOKUP(E263,commit_num_files!A$2:A$319,commit_num_files!B$2:B$319)</f>
+        <v>1</v>
+      </c>
+      <c r="I263" t="str">
+        <f>_xlfn.XLOOKUP(C263,cve_title!A$2:A$164,cve_title!B$2:B$164)</f>
+        <v>Buffer overflow in the Python bindings for the xc_vcpu_setaffinity call in Xen 4.0.x, 4.1.x, and 4.2.x allows local administrators with permissions to configure VCPU affinity to cause a denial of service (memory corruption and xend toolstack crash) and possibly gain privileges via a crafted cpumap.</v>
+      </c>
+      <c r="K263" t="s">
+        <v>1326</v>
+      </c>
+      <c r="L263" t="s">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="264" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A264" s="28" t="s">
+        <v>471</v>
+      </c>
+      <c r="B264" s="28" t="s">
+        <v>1511</v>
+      </c>
+      <c r="C264" s="28" t="s">
+        <v>472</v>
+      </c>
+      <c r="D264" s="28" t="s">
+        <v>480</v>
+      </c>
+      <c r="E264" s="29" t="s">
+        <v>473</v>
+      </c>
+      <c r="F264" s="30" t="s">
+        <v>506</v>
+      </c>
+      <c r="G264" s="29" t="s">
+        <v>504</v>
+      </c>
+      <c r="H264" s="28">
+        <f>_xlfn.XLOOKUP(E264,commit_num_files!A$2:A$319,commit_num_files!B$2:B$319)</f>
+        <v>1</v>
+      </c>
+      <c r="I264" s="28" t="str">
+        <f>_xlfn.XLOOKUP(C264,cve_title!A$2:A$164,cve_title!B$2:B$164)</f>
+        <v>The ocaml binding for the xc_vcpu_getaffinity function in Xen 4.2.x and 4.3.x frees certain memory that may still be intended for use, which allows local users to cause a denial of service (heap corruption and crash) and possibly execute arbitrary code via unspecified vectors that trigger a (1) use-after-free or (2) double free.</v>
+      </c>
+      <c r="J264" s="28"/>
+      <c r="K264" s="28" t="s">
+        <v>1327</v>
+      </c>
+      <c r="L264" s="28" t="s">
+        <v>1460</v>
+      </c>
+      <c r="M264" s="28" t="s">
+        <v>1483</v>
+      </c>
+      <c r="N264" s="28"/>
+    </row>
+    <row r="265" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A265" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="B265" s="8" t="s">
+        <v>1511</v>
+      </c>
+      <c r="C265" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="D265" s="8" t="s">
         <v>487</v>
       </c>
-      <c r="E263" s="23" t="s">
-        <v>467</v>
-      </c>
-      <c r="F263" s="24" t="s">
-        <v>506</v>
-      </c>
-      <c r="G263" s="23" t="s">
-        <v>503</v>
-      </c>
-      <c r="H263" s="22">
-        <f>_xlfn.XLOOKUP(E263,commit_num_files!A$2:A$319,commit_num_files!B$2:B$319)</f>
-        <v>1</v>
-      </c>
-      <c r="I263" s="22" t="str">
-        <f>_xlfn.XLOOKUP(C263,cve_title!A$2:A$164,cve_title!B$2:B$164)</f>
-        <v>Stack-based buffer overflow in the dirty video RAM tracking functionality in Xen 3.4 through 4.1 allows local HVM guest OS administrators to cause a denial of service (crash) via a large bitmap image.</v>
-      </c>
-      <c r="K263" s="26" t="s">
-        <v>1325</v>
-      </c>
-      <c r="L263" s="22" t="s">
+      <c r="E265" s="75" t="s">
+        <v>476</v>
+      </c>
+      <c r="F265" s="8" t="s">
+        <v>498</v>
+      </c>
+      <c r="G265" s="75" t="s">
+        <v>502</v>
+      </c>
+      <c r="H265" s="8">
+        <f>_xlfn.XLOOKUP(E265,commit_num_files!A$2:A$319,commit_num_files!B$2:B$319)</f>
+        <v>3</v>
+      </c>
+      <c r="I265" s="8" t="str">
+        <f>_xlfn.XLOOKUP(C265,cve_title!A$2:A$164,cve_title!B$2:B$164)</f>
+        <v>The Ocaml xenstored implementation (oxenstored) in Xen 4.1.x, 4.2.x, and 4.3.x allows local guest domains to cause a denial of service (domain shutdown) via a large message reply.</v>
+      </c>
+      <c r="K265" s="76" t="s">
+        <v>1520</v>
+      </c>
+      <c r="L265" s="8" t="s">
         <v>1460</v>
       </c>
-    </row>
-    <row r="264" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A264" t="s">
-        <v>468</v>
-      </c>
-      <c r="B264" t="s">
+      <c r="N265" s="8" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="266" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A266" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="B266" s="8" t="s">
         <v>1511</v>
       </c>
-      <c r="C264" t="s">
-        <v>469</v>
-      </c>
-      <c r="D264" t="s">
-        <v>491</v>
-      </c>
-      <c r="E264" s="4" t="s">
-        <v>470</v>
-      </c>
-      <c r="F264" s="9" t="s">
+      <c r="C266" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="D266" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="E266" s="75" t="s">
+        <v>476</v>
+      </c>
+      <c r="F266" s="8" t="s">
         <v>498</v>
       </c>
-      <c r="G264" s="4" t="s">
+      <c r="G266" s="75" t="s">
         <v>502</v>
       </c>
-      <c r="H264">
-        <f>_xlfn.XLOOKUP(E264,commit_num_files!A$2:A$319,commit_num_files!B$2:B$319)</f>
-        <v>1</v>
-      </c>
-      <c r="I264" t="str">
-        <f>_xlfn.XLOOKUP(C264,cve_title!A$2:A$164,cve_title!B$2:B$164)</f>
-        <v>Buffer overflow in the Python bindings for the xc_vcpu_setaffinity call in Xen 4.0.x, 4.1.x, and 4.2.x allows local administrators with permissions to configure VCPU affinity to cause a denial of service (memory corruption and xend toolstack crash) and possibly gain privileges via a crafted cpumap.</v>
-      </c>
-      <c r="K264" t="s">
-        <v>1326</v>
-      </c>
-      <c r="L264" t="s">
-        <v>1460</v>
-      </c>
-    </row>
-    <row r="265" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A265" s="28" t="s">
-        <v>471</v>
-      </c>
-      <c r="B265" s="28" t="s">
-        <v>1511</v>
-      </c>
-      <c r="C265" s="28" t="s">
-        <v>472</v>
-      </c>
-      <c r="D265" s="28" t="s">
-        <v>480</v>
-      </c>
-      <c r="E265" s="29" t="s">
-        <v>473</v>
-      </c>
-      <c r="F265" s="30" t="s">
-        <v>506</v>
-      </c>
-      <c r="G265" s="29" t="s">
-        <v>504</v>
-      </c>
-      <c r="H265" s="28">
-        <f>_xlfn.XLOOKUP(E265,commit_num_files!A$2:A$319,commit_num_files!B$2:B$319)</f>
-        <v>1</v>
-      </c>
-      <c r="I265" s="28" t="str">
-        <f>_xlfn.XLOOKUP(C265,cve_title!A$2:A$164,cve_title!B$2:B$164)</f>
-        <v>The ocaml binding for the xc_vcpu_getaffinity function in Xen 4.2.x and 4.3.x frees certain memory that may still be intended for use, which allows local users to cause a denial of service (heap corruption and crash) and possibly execute arbitrary code via unspecified vectors that trigger a (1) use-after-free or (2) double free.</v>
-      </c>
-      <c r="J265" s="28"/>
-      <c r="K265" s="28" t="s">
-        <v>1327</v>
-      </c>
-      <c r="L265" s="28" t="s">
-        <v>1460</v>
-      </c>
-      <c r="M265" s="28" t="s">
-        <v>1483</v>
-      </c>
-      <c r="N265" s="28"/>
-    </row>
-    <row r="266" spans="1:14" s="78" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A266" s="78" t="s">
-        <v>474</v>
-      </c>
-      <c r="B266" s="78" t="s">
-        <v>1511</v>
-      </c>
-      <c r="C266" s="78" t="s">
-        <v>475</v>
-      </c>
-      <c r="D266" s="78" t="s">
-        <v>487</v>
-      </c>
-      <c r="E266" s="79" t="s">
-        <v>476</v>
-      </c>
-      <c r="F266" s="78" t="s">
-        <v>498</v>
-      </c>
-      <c r="G266" s="79" t="s">
-        <v>502</v>
-      </c>
-      <c r="H266" s="78">
+      <c r="H266" s="8">
         <f>_xlfn.XLOOKUP(E266,commit_num_files!A$2:A$319,commit_num_files!B$2:B$319)</f>
         <v>3</v>
       </c>
@@ -31036,71 +31051,71 @@
         <f>_xlfn.XLOOKUP(C266,cve_title!A$2:A$164,cve_title!B$2:B$164)</f>
         <v>The Ocaml xenstored implementation (oxenstored) in Xen 4.1.x, 4.2.x, and 4.3.x allows local guest domains to cause a denial of service (domain shutdown) via a large message reply.</v>
       </c>
-      <c r="K266" s="80" t="s">
+      <c r="K266" s="76" t="s">
         <v>1520</v>
       </c>
-      <c r="L266" s="78" t="s">
+      <c r="L266" s="8" t="s">
         <v>1460</v>
       </c>
-      <c r="N266" s="78" t="s">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="267" spans="1:14" s="78" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A267" s="78" t="s">
+      <c r="N266" s="8" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="267" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A267" s="22" t="s">
         <v>474</v>
       </c>
-      <c r="B267" s="78" t="s">
+      <c r="B267" s="22" t="s">
         <v>1511</v>
       </c>
-      <c r="C267" s="78" t="s">
+      <c r="C267" s="22" t="s">
         <v>475</v>
       </c>
-      <c r="D267" s="78" t="s">
+      <c r="D267" s="22" t="s">
         <v>487</v>
       </c>
-      <c r="E267" s="79" t="s">
+      <c r="E267" s="23" t="s">
         <v>476</v>
       </c>
-      <c r="F267" s="78" t="s">
-        <v>498</v>
-      </c>
-      <c r="G267" s="79" t="s">
-        <v>502</v>
-      </c>
-      <c r="H267" s="78">
+      <c r="F267" s="24" t="s">
+        <v>506</v>
+      </c>
+      <c r="G267" s="23" t="s">
+        <v>503</v>
+      </c>
+      <c r="H267" s="22">
         <f>_xlfn.XLOOKUP(E267,commit_num_files!A$2:A$319,commit_num_files!B$2:B$319)</f>
         <v>3</v>
       </c>
-      <c r="I267" s="8" t="str">
+      <c r="I267" t="str">
         <f>_xlfn.XLOOKUP(C267,cve_title!A$2:A$164,cve_title!B$2:B$164)</f>
         <v>The Ocaml xenstored implementation (oxenstored) in Xen 4.1.x, 4.2.x, and 4.3.x allows local guest domains to cause a denial of service (domain shutdown) via a large message reply.</v>
       </c>
-      <c r="K267" s="80" t="s">
+      <c r="K267" s="26" t="s">
         <v>1520</v>
       </c>
-      <c r="L267" s="78" t="s">
+      <c r="L267" s="22" t="s">
         <v>1460</v>
       </c>
-      <c r="N267" s="78" t="s">
-        <v>1106</v>
-      </c>
-    </row>
-    <row r="268" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="N267" s="22" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="268" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A268" s="22" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="B268" s="22" t="s">
         <v>1511</v>
       </c>
       <c r="C268" s="22" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="D268" s="22" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E268" s="23" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="F268" s="24" t="s">
         <v>506</v>
@@ -31110,64 +31125,24 @@
       </c>
       <c r="H268" s="22">
         <f>_xlfn.XLOOKUP(E268,commit_num_files!A$2:A$319,commit_num_files!B$2:B$319)</f>
-        <v>3</v>
-      </c>
-      <c r="I268" t="str">
+        <v>1</v>
+      </c>
+      <c r="I268" s="28" t="str">
         <f>_xlfn.XLOOKUP(C268,cve_title!A$2:A$164,cve_title!B$2:B$164)</f>
-        <v>The Ocaml xenstored implementation (oxenstored) in Xen 4.1.x, 4.2.x, and 4.3.x allows local guest domains to cause a denial of service (domain shutdown) via a large message reply.</v>
-      </c>
+        <v>Xen 3.2.x through 4.4.x does not properly clean memory pages recovered from guests, which allows local guest OS users to obtain sensitive information via unspecified vectors.</v>
+      </c>
+      <c r="J268" s="22"/>
       <c r="K268" s="26" t="s">
-        <v>1520</v>
-      </c>
-      <c r="L268" s="22" t="s">
+        <v>1328</v>
+      </c>
+      <c r="L268" s="28" t="s">
         <v>1460</v>
       </c>
-      <c r="N268" s="22" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="269" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A269" s="22" t="s">
-        <v>477</v>
-      </c>
-      <c r="B269" s="22" t="s">
-        <v>1511</v>
-      </c>
-      <c r="C269" s="22" t="s">
-        <v>478</v>
-      </c>
-      <c r="D269" s="22" t="s">
-        <v>486</v>
-      </c>
-      <c r="E269" s="23" t="s">
-        <v>479</v>
-      </c>
-      <c r="F269" s="24" t="s">
-        <v>506</v>
-      </c>
-      <c r="G269" s="23" t="s">
-        <v>503</v>
-      </c>
-      <c r="H269" s="22">
-        <f>_xlfn.XLOOKUP(E269,commit_num_files!A$2:A$319,commit_num_files!B$2:B$319)</f>
-        <v>1</v>
-      </c>
-      <c r="I269" s="28" t="str">
-        <f>_xlfn.XLOOKUP(C269,cve_title!A$2:A$164,cve_title!B$2:B$164)</f>
-        <v>Xen 3.2.x through 4.4.x does not properly clean memory pages recovered from guests, which allows local guest OS users to obtain sensitive information via unspecified vectors.</v>
-      </c>
-      <c r="J269" s="22"/>
-      <c r="K269" s="26" t="s">
-        <v>1328</v>
-      </c>
-      <c r="L269" s="28" t="s">
-        <v>1460</v>
-      </c>
-      <c r="M269" s="22"/>
-      <c r="N269" s="22"/>
+      <c r="M268" s="22"/>
+      <c r="N268" s="22"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H269" xr:uid="{40F562BE-A651-8940-B367-6E32E546EE7D}"/>
+  <autoFilter ref="A2:H268" xr:uid="{40F562BE-A651-8940-B367-6E32E546EE7D}"/>
   <mergeCells count="1">
     <mergeCell ref="F1:G1"/>
   </mergeCells>
@@ -31177,7 +31152,7 @@
     <hyperlink ref="K6" r:id="rId2" xr:uid="{3CD0349C-16EB-B940-9059-16DC881A453B}"/>
     <hyperlink ref="K144" r:id="rId3" xr:uid="{64FE4FEB-5083-E84A-9F9F-0DA40E054D79}"/>
     <hyperlink ref="K131" r:id="rId4" xr:uid="{99FB61D0-AA30-8243-A8C9-699B7698DEDA}"/>
-    <hyperlink ref="K263" r:id="rId5" xr:uid="{676D98BD-6C2D-5841-B1ED-EC904212D2C8}"/>
+    <hyperlink ref="K262" r:id="rId5" xr:uid="{676D98BD-6C2D-5841-B1ED-EC904212D2C8}"/>
     <hyperlink ref="K132" r:id="rId6" xr:uid="{30A1C770-F282-9045-BEBE-1EA393320479}"/>
     <hyperlink ref="K191" r:id="rId7" xr:uid="{C005FF8C-17A9-0843-A40A-AF5D37E1E76F}"/>
     <hyperlink ref="K23" r:id="rId8" xr:uid="{112AED76-71EF-C34B-8E94-5CFF3186D2BE}"/>
@@ -31232,7 +31207,7 @@
     <hyperlink ref="K253" r:id="rId57" xr:uid="{1B3047BE-6841-E547-907B-E324A93DBFBE}"/>
     <hyperlink ref="K256" r:id="rId58" xr:uid="{0E9826CD-842A-BB44-833B-618B461D53DA}"/>
     <hyperlink ref="K258" r:id="rId59" xr:uid="{CA9F4555-950C-7442-8694-B0A2E8720D22}"/>
-    <hyperlink ref="K269" r:id="rId60" xr:uid="{AEBD1ECB-66D8-A541-A172-C0CF7EDA73F4}"/>
+    <hyperlink ref="K268" r:id="rId60" xr:uid="{AEBD1ECB-66D8-A541-A172-C0CF7EDA73F4}"/>
     <hyperlink ref="K238" r:id="rId61" xr:uid="{5FA90226-970E-9F4E-AF4F-6DBCC8A576EA}"/>
     <hyperlink ref="K248" r:id="rId62" xr:uid="{887A4599-0A8F-D144-AF31-394DE0486357}"/>
     <hyperlink ref="K249" r:id="rId63" xr:uid="{D24E9A65-1B62-42A9-AA15-4C71BF3B1C52}"/>
@@ -31261,9 +31236,9 @@
     <hyperlink ref="K69" r:id="rId86" xr:uid="{D90506F3-174E-4F92-BF26-95F8C05E2408}"/>
     <hyperlink ref="K105" r:id="rId87" xr:uid="{7124AA7D-416E-4AFA-9AF3-DC69820F0FA7}"/>
     <hyperlink ref="K136" r:id="rId88" xr:uid="{5F8FF057-8E3D-488A-A314-8063281FDA06}"/>
-    <hyperlink ref="K268" r:id="rId89" xr:uid="{80140301-B829-4AFF-B130-C4295EB2547F}"/>
-    <hyperlink ref="K267" r:id="rId90" xr:uid="{F4A189B1-035C-4834-93AB-5319E2CC10CF}"/>
-    <hyperlink ref="K266" r:id="rId91" xr:uid="{EBE75AE2-1F87-4CF1-8604-5E777F267CA9}"/>
+    <hyperlink ref="K267" r:id="rId89" xr:uid="{80140301-B829-4AFF-B130-C4295EB2547F}"/>
+    <hyperlink ref="K266" r:id="rId90" xr:uid="{F4A189B1-035C-4834-93AB-5319E2CC10CF}"/>
+    <hyperlink ref="K265" r:id="rId91" xr:uid="{EBE75AE2-1F87-4CF1-8604-5E777F267CA9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId92"/>

</xml_diff>